<commit_message>
Updated tare weights for envelopes
</commit_message>
<xml_diff>
--- a/Biomass_Sorting_Data.xlsx
+++ b/Biomass_Sorting_Data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="107">
   <si>
     <t>Litter</t>
   </si>
@@ -348,12 +348,6 @@
   </si>
   <si>
     <t>notes</t>
-  </si>
-  <si>
-    <t>tare_l</t>
-  </si>
-  <si>
-    <t>tare_s</t>
   </si>
 </sst>
 </file>
@@ -708,7 +702,7 @@
   <dimension ref="A1:J466"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,7 +712,7 @@
     <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>105</v>
       </c>
@@ -743,14 +737,8 @@
       <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -769,14 +757,8 @@
       <c r="F2">
         <v>10.199999999999999</v>
       </c>
-      <c r="I2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J2">
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -795,14 +777,8 @@
       <c r="F3">
         <v>7</v>
       </c>
-      <c r="I3">
-        <v>4.49</v>
-      </c>
-      <c r="J3">
-        <v>2.76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -821,14 +797,8 @@
       <c r="F4">
         <v>10.199999999999999</v>
       </c>
-      <c r="I4">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="J4">
-        <v>2.72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -847,14 +817,8 @@
       <c r="F5">
         <v>7</v>
       </c>
-      <c r="I5">
-        <v>4.47</v>
-      </c>
-      <c r="J5">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -874,7 +838,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -894,7 +858,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -911,10 +875,10 @@
         <v>8.76</v>
       </c>
       <c r="F8">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -931,10 +895,10 @@
         <v>2.97</v>
       </c>
       <c r="F9">
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2.7475000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -951,10 +915,10 @@
         <v>3.32</v>
       </c>
       <c r="F10">
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2.7475000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -971,10 +935,10 @@
         <v>9.75</v>
       </c>
       <c r="F11">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -994,7 +958,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1014,7 +978,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1031,10 +995,10 @@
         <v>3.03</v>
       </c>
       <c r="F14">
-        <v>2.77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2.7475000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1054,7 +1018,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1091,7 +1055,7 @@
         <v>3.35</v>
       </c>
       <c r="F17">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1131,7 +1095,7 @@
         <v>2.92</v>
       </c>
       <c r="F19">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1171,7 +1135,7 @@
         <v>4.07</v>
       </c>
       <c r="F21">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1231,7 +1195,7 @@
         <v>2.91</v>
       </c>
       <c r="F24">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1251,7 +1215,7 @@
         <v>2.8</v>
       </c>
       <c r="F25">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1291,7 +1255,7 @@
         <v>2.85</v>
       </c>
       <c r="F27">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1311,7 +1275,7 @@
         <v>3.22</v>
       </c>
       <c r="F28">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1331,7 +1295,7 @@
         <v>2.9</v>
       </c>
       <c r="F29">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1351,7 +1315,7 @@
         <v>2.95</v>
       </c>
       <c r="F30">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1371,7 +1335,7 @@
         <v>2.96</v>
       </c>
       <c r="F31">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1391,7 +1355,7 @@
         <v>6.6</v>
       </c>
       <c r="F32">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1408,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>104.6</v>
+        <v>104.51</v>
       </c>
       <c r="F33">
         <v>10.199999999999999</v>
@@ -1431,7 +1395,7 @@
         <v>3.77</v>
       </c>
       <c r="F34">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1451,7 +1415,7 @@
         <v>2.87</v>
       </c>
       <c r="F35">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H35" t="s">
         <v>32</v>
@@ -1474,7 +1438,7 @@
         <v>2.8</v>
       </c>
       <c r="F36">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H36" t="s">
         <v>31</v>
@@ -1497,7 +1461,7 @@
         <v>2.8</v>
       </c>
       <c r="F37">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1517,7 +1481,7 @@
         <v>3.5</v>
       </c>
       <c r="F38">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1577,7 +1541,7 @@
         <v>5.51</v>
       </c>
       <c r="F41">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1597,7 +1561,7 @@
         <v>3.12</v>
       </c>
       <c r="F42">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1637,7 +1601,7 @@
         <v>2.8</v>
       </c>
       <c r="F44">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -1697,7 +1661,7 @@
         <v>6.16</v>
       </c>
       <c r="F47">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1777,7 +1741,7 @@
         <v>2.82</v>
       </c>
       <c r="F51">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H51" t="s">
         <v>37</v>
@@ -1860,7 +1824,7 @@
         <v>3.28</v>
       </c>
       <c r="F55">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -1900,7 +1864,7 @@
         <v>6.28</v>
       </c>
       <c r="F57">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -1940,7 +1904,7 @@
         <v>3.02</v>
       </c>
       <c r="F59">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2020,7 +1984,7 @@
         <v>8.83</v>
       </c>
       <c r="F63" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -2059,10 +2023,10 @@
         <v>17</v>
       </c>
       <c r="E65">
-        <v>4.63</v>
+        <v>4.5129999999999999</v>
       </c>
       <c r="F65">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2082,7 +2046,7 @@
         <v>5.51</v>
       </c>
       <c r="F66">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -2099,10 +2063,10 @@
         <v>50</v>
       </c>
       <c r="E67">
-        <v>4.67</v>
+        <v>4.5170000000000003</v>
       </c>
       <c r="F67">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2162,7 +2126,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="F70">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -2182,7 +2146,7 @@
         <v>13.27</v>
       </c>
       <c r="F71">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2202,7 +2166,7 @@
         <v>4.76</v>
       </c>
       <c r="F72">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2242,7 +2206,7 @@
         <v>8.5500000000000007</v>
       </c>
       <c r="F74">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2259,10 +2223,10 @@
         <v>58</v>
       </c>
       <c r="E75">
-        <v>4.6100000000000003</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="F75">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G75"/>
       <c r="H75"/>
@@ -2284,7 +2248,7 @@
         <v>6.23</v>
       </c>
       <c r="F76">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2344,7 +2308,7 @@
         <v>8.27</v>
       </c>
       <c r="F79">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2364,7 +2328,7 @@
         <v>2.93</v>
       </c>
       <c r="F80">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2384,7 +2348,7 @@
         <v>2.87</v>
       </c>
       <c r="F81">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2404,7 +2368,7 @@
         <v>2.87</v>
       </c>
       <c r="F82">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2424,7 +2388,7 @@
         <v>2.81</v>
       </c>
       <c r="F83">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H83" t="s">
         <v>59</v>
@@ -2447,7 +2411,7 @@
         <v>2.84</v>
       </c>
       <c r="F84">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H84" t="s">
         <v>81</v>
@@ -2470,7 +2434,7 @@
         <v>4.3</v>
       </c>
       <c r="F85">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2510,7 +2474,7 @@
         <v>3.07</v>
       </c>
       <c r="F87">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2550,7 +2514,7 @@
         <v>2.85</v>
       </c>
       <c r="F89">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2570,7 +2534,7 @@
         <v>3.07</v>
       </c>
       <c r="F90">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2590,7 +2554,7 @@
         <v>3.07</v>
       </c>
       <c r="F91">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2610,7 +2574,7 @@
         <v>2.88</v>
       </c>
       <c r="F92">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2630,7 +2594,7 @@
         <v>2.98</v>
       </c>
       <c r="F93">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2650,7 +2614,7 @@
         <v>2.9</v>
       </c>
       <c r="F94">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -2670,7 +2634,7 @@
         <v>3.12</v>
       </c>
       <c r="F95">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -2690,7 +2654,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="F96">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -2707,10 +2671,10 @@
         <v>95</v>
       </c>
       <c r="E97">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="F97">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -2730,7 +2694,7 @@
         <v>2.83</v>
       </c>
       <c r="F98">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
@@ -2770,7 +2734,7 @@
         <v>7.08</v>
       </c>
       <c r="F100">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -2810,7 +2774,7 @@
         <v>4.7</v>
       </c>
       <c r="F102">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
@@ -2970,7 +2934,7 @@
         <v>4.96</v>
       </c>
       <c r="F110">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -2990,7 +2954,7 @@
         <v>5.64</v>
       </c>
       <c r="F111">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -3030,7 +2994,7 @@
         <v>4.49</v>
       </c>
       <c r="F113">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -3050,7 +3014,7 @@
         <v>4.5</v>
       </c>
       <c r="F114">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H114" t="s">
         <v>64</v>
@@ -3073,7 +3037,7 @@
         <v>5.17</v>
       </c>
       <c r="F115">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -3090,10 +3054,10 @@
         <v>69</v>
       </c>
       <c r="E116">
-        <v>4.67</v>
+        <v>4.5170000000000003</v>
       </c>
       <c r="F116">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -3110,10 +3074,10 @@
         <v>50</v>
       </c>
       <c r="E117">
-        <v>4.62</v>
+        <v>4.5119999999999996</v>
       </c>
       <c r="F117">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -3153,7 +3117,7 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="F119">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -3173,7 +3137,7 @@
         <v>5.07</v>
       </c>
       <c r="F120">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -3193,7 +3157,7 @@
         <v>2.83</v>
       </c>
       <c r="F121">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -3213,7 +3177,7 @@
         <v>2.98</v>
       </c>
       <c r="F122">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -3230,10 +3194,10 @@
         <v>93</v>
       </c>
       <c r="E123">
-        <v>4.66</v>
+        <v>4.516</v>
       </c>
       <c r="F123">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -3253,7 +3217,7 @@
         <v>2.99</v>
       </c>
       <c r="F124">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3273,7 +3237,7 @@
         <v>3.04</v>
       </c>
       <c r="F125">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -3293,7 +3257,7 @@
         <v>2.84</v>
       </c>
       <c r="F126">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -3333,7 +3297,7 @@
         <v>3.23</v>
       </c>
       <c r="F128">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -3353,7 +3317,7 @@
         <v>4.93</v>
       </c>
       <c r="F129">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
@@ -3373,7 +3337,7 @@
         <v>2.99</v>
       </c>
       <c r="F130">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
@@ -3393,7 +3357,7 @@
         <v>3.17</v>
       </c>
       <c r="F131">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H131" t="s">
         <v>59</v>
@@ -3416,7 +3380,7 @@
         <v>3.54</v>
       </c>
       <c r="F132">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
@@ -3436,7 +3400,7 @@
         <v>6.03</v>
       </c>
       <c r="F133">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
@@ -3476,7 +3440,7 @@
         <v>2.93</v>
       </c>
       <c r="F135">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -3496,7 +3460,7 @@
         <v>7.01</v>
       </c>
       <c r="F136">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -3516,7 +3480,7 @@
         <v>7.77</v>
       </c>
       <c r="F137">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -3536,7 +3500,7 @@
         <v>5.27</v>
       </c>
       <c r="F138">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H138" t="s">
         <v>59</v>
@@ -3579,7 +3543,7 @@
         <v>2.83</v>
       </c>
       <c r="F140">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -3599,7 +3563,7 @@
         <v>7.11</v>
       </c>
       <c r="F141">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -3619,7 +3583,7 @@
         <v>3</v>
       </c>
       <c r="F142">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -3659,7 +3623,7 @@
         <v>2.93</v>
       </c>
       <c r="F144">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -3679,7 +3643,7 @@
         <v>3.69</v>
       </c>
       <c r="F145">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -3699,7 +3663,7 @@
         <v>3.85</v>
       </c>
       <c r="F146">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
@@ -3719,7 +3683,7 @@
         <v>7.03</v>
       </c>
       <c r="F147">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -3739,7 +3703,7 @@
         <v>2.87</v>
       </c>
       <c r="F148">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H148" t="s">
         <v>59</v>
@@ -3762,7 +3726,7 @@
         <v>3.13</v>
       </c>
       <c r="F149">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H149" t="s">
         <v>59</v>
@@ -3785,7 +3749,7 @@
         <v>6.81</v>
       </c>
       <c r="F150">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -3825,7 +3789,7 @@
         <v>2.89</v>
       </c>
       <c r="F152">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -3845,7 +3809,7 @@
         <v>2.97</v>
       </c>
       <c r="F153">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -3862,10 +3826,10 @@
         <v>15</v>
       </c>
       <c r="E154">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="F154">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H154" t="s">
         <v>59</v>
@@ -3888,7 +3852,7 @@
         <v>2.83</v>
       </c>
       <c r="F155">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H155" t="s">
         <v>59</v>
@@ -3911,7 +3875,7 @@
         <v>2.87</v>
       </c>
       <c r="F156">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -3948,10 +3912,10 @@
         <v>68</v>
       </c>
       <c r="E158">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="F158">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -3971,7 +3935,7 @@
         <v>4.91</v>
       </c>
       <c r="F159">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -4011,7 +3975,7 @@
         <v>5.83</v>
       </c>
       <c r="F161">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
@@ -4051,7 +4015,7 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="F163">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
@@ -4111,7 +4075,7 @@
         <v>5.27</v>
       </c>
       <c r="F166">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
@@ -4131,7 +4095,7 @@
         <v>4.47</v>
       </c>
       <c r="F167">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H167" t="s">
         <v>59</v>
@@ -4154,7 +4118,7 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="F168">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H168" t="s">
         <v>81</v>
@@ -4177,7 +4141,7 @@
         <v>3.99</v>
       </c>
       <c r="F169">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -4197,7 +4161,7 @@
         <v>3.03</v>
       </c>
       <c r="F170">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -4217,7 +4181,7 @@
         <v>6.76</v>
       </c>
       <c r="F171">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -4257,7 +4221,7 @@
         <v>4.97</v>
       </c>
       <c r="F173">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -4317,7 +4281,7 @@
         <v>7.16</v>
       </c>
       <c r="F176">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -4337,7 +4301,7 @@
         <v>2.95</v>
       </c>
       <c r="F177">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -4377,7 +4341,7 @@
         <v>8.77</v>
       </c>
       <c r="F179">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -4397,7 +4361,7 @@
         <v>2.96</v>
       </c>
       <c r="F180">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -4557,7 +4521,7 @@
         <v>4.96</v>
       </c>
       <c r="F188">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -4574,7 +4538,7 @@
         <v>12</v>
       </c>
       <c r="E189">
-        <v>14.6</v>
+        <v>14.51</v>
       </c>
       <c r="F189">
         <v>7</v>
@@ -4617,7 +4581,7 @@
         <v>4.8899999999999997</v>
       </c>
       <c r="F191">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -4637,7 +4601,7 @@
         <v>7.03</v>
       </c>
       <c r="F192">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
@@ -4674,7 +4638,7 @@
         <v>0</v>
       </c>
       <c r="E194">
-        <v>54.6</v>
+        <v>54.51</v>
       </c>
       <c r="F194">
         <v>7</v>
@@ -4697,7 +4661,7 @@
         <v>5.0199999999999996</v>
       </c>
       <c r="F195">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G195"/>
       <c r="H195"/>
@@ -4739,7 +4703,7 @@
         <v>7.56</v>
       </c>
       <c r="F197">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
@@ -4779,7 +4743,7 @@
         <v>2.95</v>
       </c>
       <c r="F199">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
@@ -4799,7 +4763,7 @@
         <v>3.63</v>
       </c>
       <c r="F200">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
@@ -4819,7 +4783,7 @@
         <v>2.76</v>
       </c>
       <c r="F201">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H201" t="s">
         <v>59</v>
@@ -4842,7 +4806,7 @@
         <v>8.69</v>
       </c>
       <c r="F202">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
@@ -4862,7 +4826,7 @@
         <v>7.08</v>
       </c>
       <c r="F203">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
@@ -4882,7 +4846,7 @@
         <v>2.76</v>
       </c>
       <c r="F204">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
@@ -4922,7 +4886,7 @@
         <v>12.95</v>
       </c>
       <c r="F206">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
@@ -4962,7 +4926,7 @@
         <v>7.12</v>
       </c>
       <c r="F208">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
@@ -4979,10 +4943,10 @@
         <v>15</v>
       </c>
       <c r="E209">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="F209">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H209" t="s">
         <v>59</v>
@@ -5005,7 +4969,7 @@
         <v>2.85</v>
       </c>
       <c r="F210">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H210" t="s">
         <v>59</v>
@@ -5028,7 +4992,7 @@
         <v>4.88</v>
       </c>
       <c r="F211">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
@@ -5048,7 +5012,7 @@
         <v>4.72</v>
       </c>
       <c r="F212">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
@@ -5108,7 +5072,7 @@
         <v>2.75</v>
       </c>
       <c r="F215">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H215" t="s">
         <v>59</v>
@@ -5131,7 +5095,7 @@
         <v>8.39</v>
       </c>
       <c r="F216">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
@@ -5171,7 +5135,7 @@
         <v>9.2799999999999994</v>
       </c>
       <c r="F218">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.2">
@@ -5211,7 +5175,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="F220">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.2">
@@ -5231,7 +5195,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="F221">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.2">
@@ -5251,7 +5215,7 @@
         <v>5.2</v>
       </c>
       <c r="F222">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.2">
@@ -5271,7 +5235,7 @@
         <v>4.2</v>
       </c>
       <c r="F223">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.2">
@@ -5291,7 +5255,7 @@
         <v>4.74</v>
       </c>
       <c r="F224">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.2">
@@ -5351,7 +5315,7 @@
         <v>4.54</v>
       </c>
       <c r="F227">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G227"/>
       <c r="H227"/>
@@ -5373,7 +5337,7 @@
         <v>4.74</v>
       </c>
       <c r="F228">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.2">
@@ -5390,10 +5354,10 @@
         <v>27</v>
       </c>
       <c r="E229">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="F229">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.2">
@@ -5433,7 +5397,7 @@
         <v>11.97</v>
       </c>
       <c r="F231">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.2">
@@ -5450,10 +5414,10 @@
         <v>51</v>
       </c>
       <c r="E232">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="F232">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.2">
@@ -5473,7 +5437,7 @@
         <v>2.78</v>
       </c>
       <c r="F233">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.2">
@@ -5493,7 +5457,7 @@
         <v>3</v>
       </c>
       <c r="F234">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.2">
@@ -5510,10 +5474,10 @@
         <v>8</v>
       </c>
       <c r="E235">
-        <v>4.6900000000000004</v>
+        <v>4.5190000000000001</v>
       </c>
       <c r="F235">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.2">
@@ -5553,7 +5517,7 @@
         <v>5.98</v>
       </c>
       <c r="F237">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.2">
@@ -5573,7 +5537,7 @@
         <v>5.78</v>
       </c>
       <c r="F238">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H238" t="s">
         <v>61</v>
@@ -5596,7 +5560,7 @@
         <v>5.68</v>
       </c>
       <c r="F239">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -5616,7 +5580,7 @@
         <v>5.41</v>
       </c>
       <c r="F240">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
@@ -5636,7 +5600,7 @@
         <v>2.81</v>
       </c>
       <c r="F241">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
@@ -5656,7 +5620,7 @@
         <v>2.81</v>
       </c>
       <c r="F242">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
@@ -5676,7 +5640,7 @@
         <v>2.78</v>
       </c>
       <c r="F243">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H243" t="s">
         <v>59</v>
@@ -5699,7 +5663,7 @@
         <v>2.81</v>
       </c>
       <c r="F244">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H244" t="s">
         <v>59</v>
@@ -5762,7 +5726,7 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F247">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
@@ -5822,7 +5786,7 @@
         <v>7.38</v>
       </c>
       <c r="F250">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -5842,7 +5806,7 @@
         <v>5.38</v>
       </c>
       <c r="F251">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -5902,7 +5866,7 @@
         <v>6.55</v>
       </c>
       <c r="F254">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
@@ -5962,7 +5926,7 @@
         <v>9.84</v>
       </c>
       <c r="F257">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
@@ -5982,7 +5946,7 @@
         <v>11.66</v>
       </c>
       <c r="F258" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G258" s="2"/>
       <c r="H258" s="2"/>
@@ -6004,7 +5968,7 @@
         <v>6.26</v>
       </c>
       <c r="F259">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
@@ -6044,7 +6008,7 @@
         <v>4.38</v>
       </c>
       <c r="F261">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="262" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6064,7 +6028,7 @@
         <v>10.56</v>
       </c>
       <c r="F262" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.2">
@@ -6124,7 +6088,7 @@
         <v>4.76</v>
       </c>
       <c r="F265">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
@@ -6164,7 +6128,7 @@
         <v>8.44</v>
       </c>
       <c r="F267">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.2">
@@ -6204,7 +6168,7 @@
         <v>2.85</v>
       </c>
       <c r="F269">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.2">
@@ -6224,7 +6188,7 @@
         <v>2.86</v>
       </c>
       <c r="F270">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.2">
@@ -6264,7 +6228,7 @@
         <v>11.8</v>
       </c>
       <c r="F272">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
@@ -6284,7 +6248,7 @@
         <v>7.86</v>
       </c>
       <c r="F273">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
@@ -6324,7 +6288,7 @@
         <v>6.14</v>
       </c>
       <c r="F275">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
@@ -6344,7 +6308,7 @@
         <v>7.17</v>
       </c>
       <c r="F276">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
@@ -6381,10 +6345,10 @@
         <v>43</v>
       </c>
       <c r="E278">
-        <v>4.68</v>
+        <v>4.5179999999999998</v>
       </c>
       <c r="F278">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
@@ -6444,7 +6408,7 @@
         <v>3.24</v>
       </c>
       <c r="F281">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
@@ -6464,7 +6428,7 @@
         <v>3.43</v>
       </c>
       <c r="F282">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.2">
@@ -6524,7 +6488,7 @@
         <v>5.07</v>
       </c>
       <c r="F285">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.2">
@@ -6564,7 +6528,7 @@
         <v>4.74</v>
       </c>
       <c r="F287">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
@@ -6624,7 +6588,7 @@
         <v>4.7</v>
       </c>
       <c r="F290">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.2">
@@ -6684,7 +6648,7 @@
         <v>14.71</v>
       </c>
       <c r="F293">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.2">
@@ -6704,7 +6668,7 @@
         <v>6.53</v>
       </c>
       <c r="F294">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.2">
@@ -6781,10 +6745,10 @@
         <v>72</v>
       </c>
       <c r="E298">
-        <v>4.6100000000000003</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="F298">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.2">
@@ -6804,7 +6768,7 @@
         <v>4.75</v>
       </c>
       <c r="F299">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
@@ -6844,7 +6808,7 @@
         <v>8.08</v>
       </c>
       <c r="F301" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.2">
@@ -6861,10 +6825,10 @@
         <v>46</v>
       </c>
       <c r="E302">
-        <v>4.63</v>
+        <v>4.5129999999999999</v>
       </c>
       <c r="F302">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.2">
@@ -6881,10 +6845,10 @@
         <v>15</v>
       </c>
       <c r="E303">
-        <v>4.6100000000000003</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="F303">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H303" t="s">
         <v>59</v>
@@ -6947,7 +6911,7 @@
         <v>6.98</v>
       </c>
       <c r="F306">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.2">
@@ -6967,7 +6931,7 @@
         <v>5.32</v>
       </c>
       <c r="F307">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.2">
@@ -6987,7 +6951,7 @@
         <v>4.46</v>
       </c>
       <c r="F308">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.2">
@@ -7024,7 +6988,7 @@
         <v>0</v>
       </c>
       <c r="E310">
-        <v>124.6</v>
+        <v>124.51</v>
       </c>
       <c r="F310">
         <v>10.199999999999999</v>
@@ -7091,7 +7055,7 @@
         <v>4.46</v>
       </c>
       <c r="F313">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.2">
@@ -7131,7 +7095,7 @@
         <v>5.93</v>
       </c>
       <c r="F315">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.2">
@@ -7151,7 +7115,7 @@
         <v>4.87</v>
       </c>
       <c r="F316">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.2">
@@ -7171,7 +7135,7 @@
         <v>4.53</v>
       </c>
       <c r="F317">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.2">
@@ -7191,7 +7155,7 @@
         <v>11.91</v>
       </c>
       <c r="F318">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.2">
@@ -7211,7 +7175,7 @@
         <v>4.84</v>
       </c>
       <c r="F319">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.2">
@@ -7251,7 +7215,7 @@
         <v>6.3</v>
       </c>
       <c r="F321">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G321"/>
       <c r="H321"/>
@@ -7273,7 +7237,7 @@
         <v>8.19</v>
       </c>
       <c r="F322">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G322"/>
       <c r="H322"/>
@@ -7295,7 +7259,7 @@
         <v>3.09</v>
       </c>
       <c r="F323">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.2">
@@ -7315,7 +7279,7 @@
         <v>9.82</v>
       </c>
       <c r="F324">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.2">
@@ -7335,7 +7299,7 @@
         <v>5.55</v>
       </c>
       <c r="F325">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.2">
@@ -7355,7 +7319,7 @@
         <v>2.79</v>
       </c>
       <c r="F326">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H326" t="s">
         <v>59</v>
@@ -7398,7 +7362,7 @@
         <v>2.83</v>
       </c>
       <c r="F328">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H328" t="s">
         <v>49</v>
@@ -7441,7 +7405,7 @@
         <v>2.83</v>
       </c>
       <c r="F330">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="331" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7461,7 +7425,7 @@
         <v>2.82</v>
       </c>
       <c r="F331">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G331"/>
       <c r="H331"/>
@@ -7483,7 +7447,7 @@
         <v>4.72</v>
       </c>
       <c r="F332">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H332" t="s">
         <v>66</v>
@@ -7506,7 +7470,7 @@
         <v>4.54</v>
       </c>
       <c r="F333">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.2">
@@ -7546,7 +7510,7 @@
         <v>4.51</v>
       </c>
       <c r="F335">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H335" t="s">
         <v>67</v>
@@ -7569,7 +7533,7 @@
         <v>6.6</v>
       </c>
       <c r="F336">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="337" spans="1:6" x14ac:dyDescent="0.2">
@@ -7586,10 +7550,10 @@
         <v>7</v>
       </c>
       <c r="E337">
-        <v>4.6100000000000003</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="F337">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.2">
@@ -7629,7 +7593,7 @@
         <v>6.78</v>
       </c>
       <c r="F339">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.2">
@@ -7649,7 +7613,7 @@
         <v>9.67</v>
       </c>
       <c r="F340">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="341" spans="1:6" x14ac:dyDescent="0.2">
@@ -7669,7 +7633,7 @@
         <v>5.41</v>
       </c>
       <c r="F341">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.2">
@@ -7689,7 +7653,7 @@
         <v>11.19</v>
       </c>
       <c r="F342">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.2">
@@ -7709,7 +7673,7 @@
         <v>6.96</v>
       </c>
       <c r="F343">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.2">
@@ -7729,7 +7693,7 @@
         <v>5.31</v>
       </c>
       <c r="F344">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.2">
@@ -7746,10 +7710,10 @@
         <v>76</v>
       </c>
       <c r="E345">
-        <v>4.6500000000000004</v>
+        <v>4.5149999999999997</v>
       </c>
       <c r="F345">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.2">
@@ -7769,7 +7733,7 @@
         <v>7.45</v>
       </c>
       <c r="F346">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.2">
@@ -7789,7 +7753,7 @@
         <v>5.99</v>
       </c>
       <c r="F347">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="348" spans="1:6" x14ac:dyDescent="0.2">
@@ -7809,7 +7773,7 @@
         <v>9.4</v>
       </c>
       <c r="F348">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="349" spans="1:6" x14ac:dyDescent="0.2">
@@ -7849,7 +7813,7 @@
         <v>7.6</v>
       </c>
       <c r="F350">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="351" spans="1:6" x14ac:dyDescent="0.2">
@@ -7869,7 +7833,7 @@
         <v>7.1</v>
       </c>
       <c r="F351">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.2">
@@ -7909,7 +7873,7 @@
         <v>4.87</v>
       </c>
       <c r="F353">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G353"/>
       <c r="H353"/>
@@ -7931,7 +7895,7 @@
         <v>10.57</v>
       </c>
       <c r="F354">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G354"/>
       <c r="H354"/>
@@ -7953,7 +7917,7 @@
         <v>11.73</v>
       </c>
       <c r="F355">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G355"/>
       <c r="H355"/>
@@ -7997,7 +7961,7 @@
         <v>6.06</v>
       </c>
       <c r="F357">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G357"/>
       <c r="H357"/>
@@ -8019,7 +7983,7 @@
         <v>3.16</v>
       </c>
       <c r="F358">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G358"/>
       <c r="H358"/>
@@ -8041,7 +8005,7 @@
         <v>2.73</v>
       </c>
       <c r="F359">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="360" spans="1:8" x14ac:dyDescent="0.2">
@@ -8061,7 +8025,7 @@
         <v>15.58</v>
       </c>
       <c r="F360">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="361" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -8081,7 +8045,7 @@
         <v>2.74</v>
       </c>
       <c r="F361">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G361"/>
       <c r="H361" t="s">
@@ -8105,7 +8069,7 @@
         <v>2.92</v>
       </c>
       <c r="F362">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G362"/>
       <c r="H362"/>
@@ -8127,7 +8091,7 @@
         <v>8.4499999999999993</v>
       </c>
       <c r="F363">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="364" spans="1:8" x14ac:dyDescent="0.2">
@@ -8147,7 +8111,7 @@
         <v>2.91</v>
       </c>
       <c r="F364">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="365" spans="1:8" x14ac:dyDescent="0.2">
@@ -8167,7 +8131,7 @@
         <v>2.92</v>
       </c>
       <c r="F365">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="366" spans="1:8" x14ac:dyDescent="0.2">
@@ -8187,7 +8151,7 @@
         <v>5.65</v>
       </c>
       <c r="F366">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="367" spans="1:8" x14ac:dyDescent="0.2">
@@ -8207,7 +8171,7 @@
         <v>2.9</v>
       </c>
       <c r="F367">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="368" spans="1:8" x14ac:dyDescent="0.2">
@@ -8227,7 +8191,7 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="F368">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="369" spans="1:8" x14ac:dyDescent="0.2">
@@ -8247,7 +8211,7 @@
         <v>7.64</v>
       </c>
       <c r="F369">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="370" spans="1:8" x14ac:dyDescent="0.2">
@@ -8267,7 +8231,7 @@
         <v>6.73</v>
       </c>
       <c r="F370">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.2">
@@ -8287,7 +8251,7 @@
         <v>5.53</v>
       </c>
       <c r="F371">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="372" spans="1:8" x14ac:dyDescent="0.2">
@@ -8327,7 +8291,7 @@
         <v>2.84</v>
       </c>
       <c r="F373">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="374" spans="1:8" x14ac:dyDescent="0.2">
@@ -8347,7 +8311,7 @@
         <v>6.5</v>
       </c>
       <c r="F374">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="375" spans="1:8" x14ac:dyDescent="0.2">
@@ -8367,7 +8331,7 @@
         <v>2.87</v>
       </c>
       <c r="F375">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="376" spans="1:8" x14ac:dyDescent="0.2">
@@ -8387,7 +8351,7 @@
         <v>5.38</v>
       </c>
       <c r="F376">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="377" spans="1:8" x14ac:dyDescent="0.2">
@@ -8407,7 +8371,7 @@
         <v>2.89</v>
       </c>
       <c r="F377">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="378" spans="1:8" x14ac:dyDescent="0.2">
@@ -8427,7 +8391,7 @@
         <v>2.85</v>
       </c>
       <c r="F378">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="379" spans="1:8" x14ac:dyDescent="0.2">
@@ -8487,7 +8451,7 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="F381">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="382" spans="1:8" x14ac:dyDescent="0.2">
@@ -8507,7 +8471,7 @@
         <v>8.16</v>
       </c>
       <c r="F382">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="383" spans="1:8" x14ac:dyDescent="0.2">
@@ -8527,7 +8491,7 @@
         <v>6.45</v>
       </c>
       <c r="F383">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="384" spans="1:8" x14ac:dyDescent="0.2">
@@ -8547,7 +8511,7 @@
         <v>10.54</v>
       </c>
       <c r="F384" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G384" s="2"/>
       <c r="H384" s="2"/>
@@ -8569,7 +8533,7 @@
         <v>5.53</v>
       </c>
       <c r="F385">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="386" spans="1:8" x14ac:dyDescent="0.2">
@@ -8589,7 +8553,7 @@
         <v>4.57</v>
       </c>
       <c r="F386">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="387" spans="1:8" x14ac:dyDescent="0.2">
@@ -8606,10 +8570,10 @@
         <v>7</v>
       </c>
       <c r="E387">
-        <v>4.6500000000000004</v>
+        <v>4.5149999999999997</v>
       </c>
       <c r="F387">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="388" spans="1:8" x14ac:dyDescent="0.2">
@@ -8649,7 +8613,7 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="F389">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="390" spans="1:8" x14ac:dyDescent="0.2">
@@ -8666,10 +8630,10 @@
         <v>71</v>
       </c>
       <c r="E390">
-        <v>4.63</v>
+        <v>4.5129999999999999</v>
       </c>
       <c r="F390">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="391" spans="1:8" x14ac:dyDescent="0.2">
@@ -8689,7 +8653,7 @@
         <v>13.08</v>
       </c>
       <c r="F391">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="392" spans="1:8" x14ac:dyDescent="0.2">
@@ -8706,10 +8670,10 @@
         <v>46</v>
       </c>
       <c r="E392">
-        <v>4.62</v>
+        <v>4.5119999999999996</v>
       </c>
       <c r="F392">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="393" spans="1:8" x14ac:dyDescent="0.2">
@@ -8729,7 +8693,7 @@
         <v>9.31</v>
       </c>
       <c r="F393">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="394" spans="1:8" x14ac:dyDescent="0.2">
@@ -8749,7 +8713,7 @@
         <v>5.89</v>
       </c>
       <c r="F394" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G394" s="2"/>
       <c r="H394" s="2"/>
@@ -8771,7 +8735,7 @@
         <v>5.23</v>
       </c>
       <c r="F395" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G395" s="2"/>
       <c r="H395" s="2"/>
@@ -8793,7 +8757,7 @@
         <v>3.54</v>
       </c>
       <c r="F396">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="397" spans="1:8" x14ac:dyDescent="0.2">
@@ -8833,7 +8797,7 @@
         <v>7.22</v>
       </c>
       <c r="F398">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="399" spans="1:8" x14ac:dyDescent="0.2">
@@ -8853,7 +8817,7 @@
         <v>3.07</v>
       </c>
       <c r="F399">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="400" spans="1:8" x14ac:dyDescent="0.2">
@@ -8873,7 +8837,7 @@
         <v>8.14</v>
       </c>
       <c r="F400">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="401" spans="1:8" x14ac:dyDescent="0.2">
@@ -8913,7 +8877,7 @@
         <v>2.79</v>
       </c>
       <c r="F402">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.2">
@@ -8933,7 +8897,7 @@
         <v>6.62</v>
       </c>
       <c r="F403">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.2">
@@ -8953,7 +8917,7 @@
         <v>3.2</v>
       </c>
       <c r="F404">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.2">
@@ -8993,7 +8957,7 @@
         <v>2.97</v>
       </c>
       <c r="F406">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.2">
@@ -9013,7 +8977,7 @@
         <v>3.64</v>
       </c>
       <c r="F407">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.2">
@@ -9033,7 +8997,7 @@
         <v>3.04</v>
       </c>
       <c r="F408">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.2">
@@ -9053,7 +9017,7 @@
         <v>2.96</v>
       </c>
       <c r="F409">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.2">
@@ -9073,7 +9037,7 @@
         <v>3.03</v>
       </c>
       <c r="F410">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="411" spans="1:8" x14ac:dyDescent="0.2">
@@ -9093,7 +9057,7 @@
         <v>3.31</v>
       </c>
       <c r="F411">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.2">
@@ -9133,7 +9097,7 @@
         <v>3.07</v>
       </c>
       <c r="F413">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.2">
@@ -9173,7 +9137,7 @@
         <v>2.82</v>
       </c>
       <c r="F415">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H415" t="s">
         <v>29</v>
@@ -9196,7 +9160,7 @@
         <v>2.84</v>
       </c>
       <c r="F416">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="417" spans="1:10" x14ac:dyDescent="0.2">
@@ -9216,7 +9180,7 @@
         <v>5.57</v>
       </c>
       <c r="F417">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="418" spans="1:10" x14ac:dyDescent="0.2">
@@ -9236,7 +9200,7 @@
         <v>4.58</v>
       </c>
       <c r="F418">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="419" spans="1:10" x14ac:dyDescent="0.2">
@@ -9256,7 +9220,7 @@
         <v>4.8099999999999996</v>
       </c>
       <c r="F419">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="420" spans="1:10" x14ac:dyDescent="0.2">
@@ -9273,7 +9237,7 @@
         <v>0</v>
       </c>
       <c r="E420">
-        <v>34.6</v>
+        <v>34.51</v>
       </c>
       <c r="F420">
         <v>7</v>
@@ -9296,7 +9260,7 @@
         <v>5.12</v>
       </c>
       <c r="F421">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="422" spans="1:10" x14ac:dyDescent="0.2">
@@ -9313,10 +9277,10 @@
         <v>35</v>
       </c>
       <c r="E422">
-        <v>4.6500000000000004</v>
+        <v>4.5149999999999997</v>
       </c>
       <c r="F422">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="423" spans="1:10" x14ac:dyDescent="0.2">
@@ -9336,7 +9300,7 @@
         <v>11.59</v>
       </c>
       <c r="F423">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="424" spans="1:10" x14ac:dyDescent="0.2">
@@ -9356,7 +9320,7 @@
         <v>4.54</v>
       </c>
       <c r="F424">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="425" spans="1:10" x14ac:dyDescent="0.2">
@@ -9373,10 +9337,10 @@
         <v>15</v>
       </c>
       <c r="E425">
-        <v>4.6100000000000003</v>
+        <v>4.5110000000000001</v>
       </c>
       <c r="F425">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H425" t="s">
         <v>59</v>
@@ -9439,7 +9403,7 @@
         <v>2.91</v>
       </c>
       <c r="F428" s="2">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G428" s="2"/>
       <c r="H428" s="2"/>
@@ -9485,7 +9449,7 @@
         <v>3.51</v>
       </c>
       <c r="F430" s="2">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G430" s="2"/>
       <c r="H430" s="2"/>
@@ -9507,7 +9471,7 @@
         <v>3.01</v>
       </c>
       <c r="F431">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="432" spans="1:10" x14ac:dyDescent="0.2">
@@ -9527,7 +9491,7 @@
         <v>2.82</v>
       </c>
       <c r="F432">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="433" spans="1:10" x14ac:dyDescent="0.2">
@@ -9547,7 +9511,7 @@
         <v>3.04</v>
       </c>
       <c r="F433" s="2">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G433" s="2"/>
     </row>
@@ -9568,7 +9532,7 @@
         <v>2.89</v>
       </c>
       <c r="F434">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="435" spans="1:10" x14ac:dyDescent="0.2">
@@ -9588,7 +9552,7 @@
         <v>2.81</v>
       </c>
       <c r="F435">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="436" spans="1:10" x14ac:dyDescent="0.2">
@@ -9608,7 +9572,7 @@
         <v>5.39</v>
       </c>
       <c r="F436">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="437" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -9628,7 +9592,7 @@
         <v>3.01</v>
       </c>
       <c r="F437">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G437"/>
       <c r="H437"/>
@@ -9652,7 +9616,7 @@
         <v>3.21</v>
       </c>
       <c r="F438" s="2">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="439" spans="1:10" x14ac:dyDescent="0.2">
@@ -9694,7 +9658,7 @@
         <v>5.3</v>
       </c>
       <c r="F440" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G440" s="2"/>
       <c r="H440" s="2"/>
@@ -9757,7 +9721,7 @@
         <v>8.77</v>
       </c>
       <c r="F443" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G443" s="2"/>
       <c r="H443" s="2"/>
@@ -9779,7 +9743,7 @@
         <v>2.86</v>
       </c>
       <c r="F444" s="2">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="G444" s="2"/>
       <c r="H444" s="2"/>
@@ -9823,7 +9787,7 @@
         <v>6.84</v>
       </c>
       <c r="F446" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="G446" s="2"/>
       <c r="H446" s="2"/>
@@ -9845,7 +9809,7 @@
         <v>5.07</v>
       </c>
       <c r="F447" s="2">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="448" spans="1:10" x14ac:dyDescent="0.2">
@@ -9885,7 +9849,7 @@
         <v>5.85</v>
       </c>
       <c r="F449">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="450" spans="1:8" x14ac:dyDescent="0.2">
@@ -9905,7 +9869,7 @@
         <v>8.9499999999999993</v>
       </c>
       <c r="F450">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="451" spans="1:8" x14ac:dyDescent="0.2">
@@ -9925,7 +9889,7 @@
         <v>6.07</v>
       </c>
       <c r="F451">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="452" spans="1:8" x14ac:dyDescent="0.2">
@@ -9942,10 +9906,10 @@
         <v>54</v>
       </c>
       <c r="E452">
-        <v>4.67</v>
+        <v>4.5170000000000003</v>
       </c>
       <c r="F452">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="453" spans="1:8" x14ac:dyDescent="0.2">
@@ -9965,7 +9929,7 @@
         <v>4.84</v>
       </c>
       <c r="F453">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
       <c r="H453" t="s">
         <v>59</v>
@@ -10028,7 +9992,7 @@
         <v>3.24</v>
       </c>
       <c r="F456">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="457" spans="1:8" x14ac:dyDescent="0.2">
@@ -10048,7 +10012,7 @@
         <v>7.26</v>
       </c>
       <c r="F457">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="458" spans="1:8" x14ac:dyDescent="0.2">
@@ -10068,7 +10032,7 @@
         <v>6.05</v>
       </c>
       <c r="F458">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="459" spans="1:8" x14ac:dyDescent="0.2">
@@ -10088,7 +10052,7 @@
         <v>6.06</v>
       </c>
       <c r="F459">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="460" spans="1:8" x14ac:dyDescent="0.2">
@@ -10128,7 +10092,7 @@
         <v>3.39</v>
       </c>
       <c r="F461">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.2">
@@ -10148,7 +10112,7 @@
         <v>3.31</v>
       </c>
       <c r="F462">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.2">
@@ -10188,7 +10152,7 @@
         <v>7.67</v>
       </c>
       <c r="F464">
-        <v>4.5999999999999996</v>
+        <v>4.51</v>
       </c>
     </row>
     <row r="465" spans="1:8" x14ac:dyDescent="0.2">
@@ -10208,7 +10172,7 @@
         <v>4.22</v>
       </c>
       <c r="F465">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
     </row>
     <row r="466" spans="1:8" x14ac:dyDescent="0.2">
@@ -10228,7 +10192,7 @@
         <v>2.83</v>
       </c>
       <c r="F466">
-        <v>2.77</v>
+        <v>2.7475000000000001</v>
       </c>
       <c r="H466" t="s">
         <v>59</v>

</xml_diff>